<commit_message>
Se sube codigo nuevo actualizado funcionando y que servira como base para futuras automatizaciones
</commit_message>
<xml_diff>
--- a/Revisión-Precios-API/Dealers.xlsx
+++ b/Revisión-Precios-API/Dealers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvelasc2\source\repos\MazdaMX2\MazdaMX2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvelasc2\source\repos\Revisión-Precios-API\Revisión-Precios-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F5666B-0994-4285-B2BB-574B777AD08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84085E3-E82E-4D0F-B5D2-ED825EAF0DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="118">
   <si>
     <t>VERIFICAR</t>
   </si>
@@ -193,9 +193,6 @@
     <t>MAZDA CX-30</t>
   </si>
   <si>
-    <t>519,900</t>
-  </si>
-  <si>
     <t>MAZDA CX-5</t>
   </si>
   <si>
@@ -250,9 +247,6 @@
     <t>137</t>
   </si>
   <si>
-    <t>495,900</t>
-  </si>
-  <si>
     <t>Signature MHEV</t>
   </si>
   <si>
@@ -265,9 +259,6 @@
     <t>3.3L</t>
   </si>
   <si>
-    <t>619,900</t>
-  </si>
-  <si>
     <t>mazda-cx-70-lateral-inclinado-v2</t>
   </si>
   <si>
@@ -283,24 +274,6 @@
     <t>332</t>
   </si>
   <si>
-    <t>453,900</t>
-  </si>
-  <si>
-    <t>563,900</t>
-  </si>
-  <si>
-    <t>815,900</t>
-  </si>
-  <si>
-    <t>436,900</t>
-  </si>
-  <si>
-    <t>466,900</t>
-  </si>
-  <si>
-    <t>512,900</t>
-  </si>
-  <si>
     <t>552,900</t>
   </si>
   <si>
@@ -310,24 +283,6 @@
     <t>mazda-cx-50-flydown-v2</t>
   </si>
   <si>
-    <t>295,900</t>
-  </si>
-  <si>
-    <t>325,900</t>
-  </si>
-  <si>
-    <t>365,900</t>
-  </si>
-  <si>
-    <t>395,900</t>
-  </si>
-  <si>
-    <t>386,900</t>
-  </si>
-  <si>
-    <t>416,900</t>
-  </si>
-  <si>
     <t>mazda-mazda2-sedan-rojo-perfil-v1</t>
   </si>
   <si>
@@ -337,37 +292,88 @@
     <t>mazda-mexico-cx-3-flydown-perfil-v1</t>
   </si>
   <si>
-    <t>548,900</t>
-  </si>
-  <si>
-    <t>608,900</t>
-  </si>
-  <si>
-    <t>678,900</t>
-  </si>
-  <si>
     <t>mazda3-sedan-flydown-perfil-v2</t>
   </si>
   <si>
-    <t>397,900</t>
-  </si>
-  <si>
-    <t>437,900</t>
-  </si>
-  <si>
-    <t>477,900</t>
-  </si>
-  <si>
-    <t>547,900</t>
-  </si>
-  <si>
-    <t>958,000</t>
-  </si>
-  <si>
     <t>mazda-cx-90-flydown-rojo-artesano-inclinado-v1.png</t>
   </si>
   <si>
-    <t>1,058,000</t>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>1,061,000</t>
+  </si>
+  <si>
+    <t>300,900</t>
+  </si>
+  <si>
+    <t>330,900</t>
+  </si>
+  <si>
+    <t>370,900</t>
+  </si>
+  <si>
+    <t>398,900</t>
+  </si>
+  <si>
+    <t>403,900</t>
+  </si>
+  <si>
+    <t>442,900</t>
+  </si>
+  <si>
+    <t>482,900</t>
+  </si>
+  <si>
+    <t>458,900</t>
+  </si>
+  <si>
+    <t>498,900</t>
+  </si>
+  <si>
+    <t>568,900</t>
+  </si>
+  <si>
+    <t>391,900</t>
+  </si>
+  <si>
+    <t>421,900</t>
+  </si>
+  <si>
+    <t>441,900</t>
+  </si>
+  <si>
+    <t>471,900</t>
+  </si>
+  <si>
+    <t>517,900</t>
+  </si>
+  <si>
+    <t>557,900</t>
+  </si>
+  <si>
+    <t>551,900</t>
+  </si>
+  <si>
+    <t>611,900</t>
+  </si>
+  <si>
+    <t>681,900</t>
+  </si>
+  <si>
+    <t>818,900</t>
+  </si>
+  <si>
+    <t>961,000</t>
+  </si>
+  <si>
+    <t>529,900</t>
+  </si>
+  <si>
+    <t>629,900</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -693,7 +699,7 @@
   <dimension ref="A1:AJ13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
@@ -730,7 +736,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -833,14 +839,14 @@
       </c>
     </row>
     <row r="2" spans="1:36">
-      <c r="A2" t="b">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>117</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
         <v>35</v>
@@ -855,7 +861,7 @@
         <v>37</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>38</v>
@@ -870,7 +876,7 @@
         <v>41</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>38</v>
@@ -885,7 +891,7 @@
         <v>49</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>38</v>
@@ -900,27 +906,27 @@
         <v>50</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="X2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y2" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:36">
-      <c r="A3" t="b">
-        <v>0</v>
+      <c r="A3" t="s">
+        <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
         <v>35</v>
@@ -935,7 +941,7 @@
         <v>41</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>38</v>
@@ -950,7 +956,7 @@
         <v>49</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>38</v>
@@ -965,13 +971,13 @@
         <v>50</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="S3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T3" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>48</v>
@@ -981,14 +987,14 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:36">
-      <c r="A4" t="b">
-        <v>0</v>
+      <c r="A4" t="s">
+        <v>92</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
         <v>44</v>
@@ -1003,7 +1009,7 @@
         <v>37</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>45</v>
@@ -1018,7 +1024,7 @@
         <v>41</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>45</v>
@@ -1033,7 +1039,7 @@
         <v>49</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>45</v>
@@ -1048,7 +1054,7 @@
         <v>50</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="X4" s="1" t="s">
         <v>51</v>
@@ -1067,14 +1073,14 @@
       <c r="AI4" s="1"/>
     </row>
     <row r="5" spans="1:36">
-      <c r="A5" t="b">
-        <v>0</v>
+      <c r="A5" t="s">
+        <v>92</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
         <v>44</v>
@@ -1089,7 +1095,7 @@
         <v>41</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>45</v>
@@ -1104,7 +1110,7 @@
         <v>49</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>45</v>
@@ -1119,7 +1125,7 @@
         <v>50</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>51</v>
@@ -1137,14 +1143,14 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:36">
-      <c r="A6" t="b">
-        <v>0</v>
+      <c r="A6" t="s">
+        <v>92</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
         <v>53</v>
@@ -1159,7 +1165,7 @@
         <v>37</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>47</v>
@@ -1174,7 +1180,7 @@
         <v>41</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>47</v>
@@ -1191,14 +1197,14 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:36">
-      <c r="A7" t="b">
-        <v>0</v>
+      <c r="A7" t="s">
+        <v>92</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
         <v>56</v>
@@ -1213,7 +1219,7 @@
         <v>37</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>45</v>
@@ -1228,7 +1234,7 @@
         <v>41</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>45</v>
@@ -1243,7 +1249,7 @@
         <v>49</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>45</v>
@@ -1258,7 +1264,7 @@
         <v>50</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="X7" s="1" t="s">
         <v>51</v>
@@ -1271,17 +1277,17 @@
       </c>
     </row>
     <row r="8" spans="1:36">
-      <c r="A8" t="b">
-        <v>0</v>
+      <c r="A8" t="s">
+        <v>92</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
         <v>54</v>
@@ -1293,10 +1299,10 @@
         <v>41</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>45</v>
@@ -1308,10 +1314,10 @@
         <v>49</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>45</v>
@@ -1323,7 +1329,7 @@
         <v>50</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>51</v>
@@ -1340,17 +1346,17 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:36">
-      <c r="A9" t="b">
-        <v>0</v>
+      <c r="A9" t="s">
+        <v>92</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
         <v>54</v>
@@ -1362,10 +1368,10 @@
         <v>50</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>52</v>
@@ -1375,17 +1381,17 @@
       </c>
     </row>
     <row r="10" spans="1:36">
-      <c r="A10" t="b">
-        <v>0</v>
+      <c r="A10" t="s">
+        <v>92</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E10" t="s">
         <v>54</v>
@@ -1397,30 +1403,30 @@
         <v>42</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:36">
-      <c r="A11" t="b">
-        <v>1</v>
+      <c r="A11" t="s">
+        <v>92</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
         <v>54</v>
@@ -1429,86 +1435,86 @@
         <v>2025</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I11" s="3" t="s">
+      <c r="K11" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:36">
-      <c r="A12" t="b">
-        <v>0</v>
+      <c r="A12" t="s">
+        <v>92</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
         <v>54</v>
       </c>
       <c r="F12">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="G12" t="s">
         <v>41</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>57</v>
+        <v>115</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:36">
-      <c r="A13" t="b">
-        <v>0</v>
+      <c r="A13" t="s">
+        <v>92</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
         <v>54</v>
       </c>
       <c r="F13">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="G13" t="s">
         <v>49</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Se depura codigo para que solo revise precios desde API, se quita codigo basura.
</commit_message>
<xml_diff>
--- a/Revisión-Precios-API/Dealers.xlsx
+++ b/Revisión-Precios-API/Dealers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvelasc2\source\repos\Revisión-Precios-API\Revisión-Precios-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84085E3-E82E-4D0F-B5D2-ED825EAF0DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D5CE17-E3F6-4BDA-80D5-9D925C8F4685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="390" windowWidth="28800" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="123">
   <si>
     <t>VERIFICAR</t>
   </si>
@@ -259,9 +259,6 @@
     <t>3.3L</t>
   </si>
   <si>
-    <t>mazda-cx-70-lateral-inclinado-v2</t>
-  </si>
-  <si>
     <t>MAZDA CX-70</t>
   </si>
   <si>
@@ -373,7 +370,25 @@
     <t>629,900</t>
   </si>
   <si>
-    <t>False</t>
+    <t>mazda-cx-70-racks-flydown-inclinado-v1</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>PICKUPS</t>
+  </si>
+  <si>
+    <t>MAZDA BT-50</t>
+  </si>
+  <si>
+    <t>mazda-bt-50-roja-flydown-inclinado-v2</t>
+  </si>
+  <si>
+    <t>3.0L</t>
+  </si>
+  <si>
+    <t>829,900</t>
   </si>
 </sst>
 </file>
@@ -696,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ13"/>
+  <dimension ref="A1:AJ14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
@@ -843,7 +858,7 @@
         <v>117</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>64</v>
@@ -861,7 +876,7 @@
         <v>37</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>38</v>
@@ -876,7 +891,7 @@
         <v>41</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>38</v>
@@ -891,7 +906,7 @@
         <v>49</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>38</v>
@@ -906,7 +921,7 @@
         <v>50</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>73</v>
@@ -923,7 +938,7 @@
         <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>64</v>
@@ -941,7 +956,7 @@
         <v>41</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>38</v>
@@ -956,7 +971,7 @@
         <v>49</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>38</v>
@@ -971,7 +986,7 @@
         <v>50</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>73</v>
@@ -988,10 +1003,10 @@
     </row>
     <row r="4" spans="1:36">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>64</v>
@@ -1009,7 +1024,7 @@
         <v>37</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>45</v>
@@ -1024,7 +1039,7 @@
         <v>41</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>45</v>
@@ -1039,7 +1054,7 @@
         <v>49</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>45</v>
@@ -1054,7 +1069,7 @@
         <v>50</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="X4" s="1" t="s">
         <v>51</v>
@@ -1074,10 +1089,10 @@
     </row>
     <row r="5" spans="1:36">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>64</v>
@@ -1095,7 +1110,7 @@
         <v>41</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>45</v>
@@ -1110,7 +1125,7 @@
         <v>49</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>45</v>
@@ -1125,7 +1140,7 @@
         <v>50</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>51</v>
@@ -1144,10 +1159,10 @@
     </row>
     <row r="6" spans="1:36">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>65</v>
@@ -1165,7 +1180,7 @@
         <v>37</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>47</v>
@@ -1180,7 +1195,7 @@
         <v>41</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>47</v>
@@ -1198,10 +1213,10 @@
     </row>
     <row r="7" spans="1:36">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>65</v>
@@ -1219,7 +1234,7 @@
         <v>37</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>45</v>
@@ -1234,7 +1249,7 @@
         <v>41</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>45</v>
@@ -1249,7 +1264,7 @@
         <v>49</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>45</v>
@@ -1264,7 +1279,7 @@
         <v>50</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X7" s="1" t="s">
         <v>51</v>
@@ -1278,7 +1293,7 @@
     </row>
     <row r="8" spans="1:36">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>70</v>
@@ -1299,7 +1314,7 @@
         <v>41</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>58</v>
@@ -1314,7 +1329,7 @@
         <v>49</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>58</v>
@@ -1329,7 +1344,7 @@
         <v>50</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>51</v>
@@ -1347,10 +1362,10 @@
     </row>
     <row r="9" spans="1:36">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>65</v>
@@ -1368,7 +1383,7 @@
         <v>50</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>59</v>
@@ -1382,16 +1397,16 @@
     </row>
     <row r="10" spans="1:36">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
         <v>54</v>
@@ -1403,13 +1418,13 @@
         <v>42</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>78</v>
@@ -1417,10 +1432,10 @@
     </row>
     <row r="11" spans="1:36">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>65</v>
@@ -1438,7 +1453,7 @@
         <v>75</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>76</v>
@@ -1452,16 +1467,16 @@
     </row>
     <row r="12" spans="1:36">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" t="s">
-        <v>60</v>
+        <v>118</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="E12" t="s">
         <v>54</v>
@@ -1469,34 +1484,34 @@
       <c r="F12">
         <v>2025</v>
       </c>
-      <c r="G12" t="s">
-        <v>41</v>
+      <c r="G12" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>48</v>
+        <v>122</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:36">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
         <v>54</v>
@@ -1505,10 +1520,10 @@
         <v>2025</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>61</v>
@@ -1517,6 +1532,41 @@
         <v>62</v>
       </c>
       <c r="K13" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36">
+      <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14">
+        <v>2025</v>
+      </c>
+      <c r="G14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se suben actualizaciones de codigo
</commit_message>
<xml_diff>
--- a/Revisión-Precios-API/Dealers.xlsx
+++ b/Revisión-Precios-API/Dealers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvelasc2\source\repos\Revisión-Precios-API\Revisión-Precios-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D5CE17-E3F6-4BDA-80D5-9D925C8F4685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14891710-0B00-45D2-ABF6-E0CE2F6326CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="390" windowWidth="28800" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="127">
   <si>
     <t>VERIFICAR</t>
   </si>
@@ -389,6 +389,18 @@
   </si>
   <si>
     <t>829,900</t>
+  </si>
+  <si>
+    <t>mazda-mx-5-35-aniversario-flydown-perspectiva-v1</t>
+  </si>
+  <si>
+    <t>MAZDA MX-5 35° ANIVERSARIO</t>
+  </si>
+  <si>
+    <t>639,900</t>
+  </si>
+  <si>
+    <t>35° ANIVERSARIO</t>
   </si>
 </sst>
 </file>
@@ -711,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ14"/>
+  <dimension ref="A1:AJ15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
@@ -722,7 +734,7 @@
     <col min="1" max="1" width="12.75" customWidth="1"/>
     <col min="2" max="2" width="30.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.75" customWidth="1"/>
-    <col min="4" max="4" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.75" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="13.25" customWidth="1"/>
@@ -1570,6 +1582,41 @@
         <v>48</v>
       </c>
     </row>
+    <row r="15" spans="1:36">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15">
+        <v>2025</v>
+      </c>
+      <c r="G15" t="s">
+        <v>126</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>